<commit_message>
Updated Generate Yearly Report
</commit_message>
<xml_diff>
--- a/GenerateYearlyReport/Data/Config.xlsx
+++ b/GenerateYearlyReport/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karis\OneDrive\Documents\GitHub\UiPath-Work\GenerateYearlyReport\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karis\OneDrive\Documents\GitHub\UiPath-Training\GenerateYearlyReport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1D9B54-EBC6-4C63-AA57-18859F4DCEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F31AB3F-F3B4-4ED9-9186-1F4996846EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>WorkItems3</t>
+  </si>
+  <si>
+    <t>ReportsDownloadFilePath</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>MonthlyReports</t>
   </si>
 </sst>
 </file>
@@ -553,7 +562,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -652,11 +661,21 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13">
+        <v>2021</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Improved Upload Yearly Report and Generate Yearly Report component functionality.
</commit_message>
<xml_diff>
--- a/GenerateYearlyReport/Data/Config.xlsx
+++ b/GenerateYearlyReport/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karis\OneDrive\Documents\GitHub\UiPath-Training\GenerateYearlyReport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F31AB3F-F3B4-4ED9-9186-1F4996846EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF942E8-45F2-4446-ADF4-93A5C61933E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>MonthlyReports</t>
+  </si>
+  <si>
+    <t>YearlyReportsDownloadFilePath</t>
+  </si>
+  <si>
+    <t>YearlyReports</t>
   </si>
 </sst>
 </file>
@@ -562,7 +568,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -678,7 +684,14 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>